<commit_message>
updated testing excel file
</commit_message>
<xml_diff>
--- a/test/excel_test.xlsx
+++ b/test/excel_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Coding\Python\Scripts\easierexcel\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Coding\Python\Packages\easierexcel\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA774B1-9D9E-4BB9-9DD7-52348B813B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A087F7-1511-4034-AEF7-32F4677423D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="228" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4500" yWindow="10875" windowWidth="9870" windowHeight="7875" tabRatio="228" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -870,10 +870,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,7 +900,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="8">
         <v>31</v>
@@ -908,56 +908,34 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="8">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="8">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" s="8">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="8">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="8">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated test excel file
</commit_message>
<xml_diff>
--- a/test/excel_test.xlsx
+++ b/test/excel_test.xlsx
@@ -1,50 +1,134 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Coding\Python\Packages\easierexcel\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE16771A-8A62-4D38-93CF-95CE6A17234E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-4500" yWindow="10875" windowWidth="9870" windowHeight="7875" tabRatio="228" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet 2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Links" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="181029" fullCalcOnLoad="1"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Birth Month</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Brian</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>Allison</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>Rob</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Untouched Site Text</t>
+  </si>
+  <si>
+    <t>Tony Stark</t>
+  </si>
+  <si>
+    <t>"=HYPERLINK("https://www.Stark.com/","Website")"</t>
+  </si>
+  <si>
+    <t>Birth Year</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="16"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <sz val="8"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -115,46 +199,63 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="17">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
@@ -184,7 +285,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.7999816888943144"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -210,11 +311,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="4" tint="-0.249946592608417"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.7999816888943144"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -224,7 +325,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="-0.249946592608417"/>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -234,13 +335,13 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.249946592608417"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.7999816888943144"/>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="0.79998168889431442"/>
       </font>
       <fill>
         <patternFill>
@@ -260,7 +361,7 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="9" tint="0.7999816888943144"/>
+        <color theme="9" tint="0.79998168889431442"/>
       </font>
       <fill>
         <patternFill>
@@ -294,7 +395,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.7999816888943144"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -320,11 +421,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="4" tint="-0.249946592608417"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.7999816888943144"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -334,7 +435,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="-0.249946592608417"/>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -344,13 +445,13 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.249946592608417"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.7999816888943144"/>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="0.79998168889431442"/>
       </font>
       <fill>
         <patternFill>
@@ -370,7 +471,7 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="9" tint="0.7999816888943144"/>
+        <color theme="9" tint="0.79998168889431442"/>
       </font>
       <fill>
         <patternFill>
@@ -380,74 +481,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -713,136 +754,124 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="8.85546875" customWidth="1" style="3" min="1" max="1"/>
-    <col width="54.28515625" customWidth="1" style="4" min="2" max="2"/>
-    <col width="9.28515625" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
-    <col width="9.140625" customWidth="1" style="2" min="4" max="233"/>
-    <col width="9.140625" customWidth="1" style="2" min="234" max="16384"/>
+    <col min="1" max="1" width="8.85546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="21" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="236" width="9.140625" style="2" customWidth="1"/>
+    <col min="237" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="72" customFormat="1" customHeight="1" s="1" thickBot="1">
-      <c r="A1" s="7" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="6" t="inlineStr">
-        <is>
-          <t>Birth Month</t>
-        </is>
-      </c>
-      <c r="C1" s="9" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="10" t="inlineStr">
-        <is>
-          <t>Michael</t>
-        </is>
-      </c>
-      <c r="B2" s="11" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
-      <c r="C2" s="8" t="n">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="13">
+        <v>1991</v>
+      </c>
+      <c r="D2" s="8">
         <v>31</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="10" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
-      <c r="B3" s="11" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-      <c r="C3" s="8" t="n">
+    <row r="3" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="13">
+        <v>1990</v>
+      </c>
+      <c r="D3" s="8">
         <v>32</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="10" t="inlineStr">
-        <is>
-          <t>Brian</t>
-        </is>
-      </c>
-      <c r="B4" s="11" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-      <c r="C4" s="8" t="n">
+    <row r="4" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="13">
+        <v>1989</v>
+      </c>
+      <c r="D4" s="8">
         <v>33</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="10" t="inlineStr">
-        <is>
-          <t>Allison</t>
-        </is>
-      </c>
-      <c r="B5" s="11" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-      <c r="C5" s="8" t="n">
+    <row r="5" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="13">
+        <v>1988</v>
+      </c>
+      <c r="D5" s="8">
         <v>34</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="10" t="inlineStr">
-        <is>
-          <t>Daniel</t>
-        </is>
-      </c>
-      <c r="B6" s="11" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
-      <c r="C6" s="8" t="n">
+    <row r="6" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="13">
+        <v>1987</v>
+      </c>
+      <c r="D6" s="8">
         <v>35</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="10" t="inlineStr">
-        <is>
-          <t>Rob</t>
-        </is>
-      </c>
-      <c r="B7" s="11" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-      <c r="C7" s="8" t="n">
+    <row r="7" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="13">
+        <v>1986</v>
+      </c>
+      <c r="D7" s="8">
         <v>36</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1"/>
+  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="colorScale" priority="60">
       <colorScale>
@@ -855,39 +884,39 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" priority="27" operator="equal" dxfId="10">
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="21" priority="27" operator="equal">
       <formula>"Endless"</formula>
     </cfRule>
-    <cfRule type="containsText" priority="38" operator="containsText" dxfId="9" text="Removed">
-      <formula>NOT(ISERROR(SEARCH("Removed",C1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="42" operator="containsText" dxfId="8" text="Software">
-      <formula>NOT(ISERROR(SEARCH("Software",C1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="44" operator="containsText" dxfId="7" text="Demo">
-      <formula>NOT(ISERROR(SEARCH("Demo",C1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="45" operator="containsText" dxfId="6" text="Waiting">
-      <formula>NOT(ISERROR(SEARCH("Waiting",C1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="46" operator="containsText" dxfId="5" text="Unplayed">
-      <formula>NOT(ISERROR(SEARCH("Unplayed",C1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="47" operator="containsText" dxfId="3" text="Playing">
-      <formula>NOT(ISERROR(SEARCH("Playing",C1)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" priority="48" operator="beginsWith" dxfId="3" text="Played">
-      <formula>LEFT(C1,LEN("Played"))="Played"</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="49" operator="containsText" dxfId="2" text="Ignore">
-      <formula>NOT(ISERROR(SEARCH("Ignore",C1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="50" operator="containsText" dxfId="1" text="Finished">
-      <formula>NOT(ISERROR(SEARCH("Finished",C1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="51" operator="containsText" dxfId="0" text="Quit">
-      <formula>NOT(ISERROR(SEARCH("Quit",C1)))</formula>
+    <cfRule type="containsText" dxfId="20" priority="38" operator="containsText" text="Removed">
+      <formula>NOT(ISERROR(SEARCH("Removed",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="42" operator="containsText" text="Software">
+      <formula>NOT(ISERROR(SEARCH("Software",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="44" operator="containsText" text="Demo">
+      <formula>NOT(ISERROR(SEARCH("Demo",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="45" operator="containsText" text="Waiting">
+      <formula>NOT(ISERROR(SEARCH("Waiting",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="46" operator="containsText" text="Unplayed">
+      <formula>NOT(ISERROR(SEARCH("Unplayed",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="47" operator="containsText" text="Playing">
+      <formula>NOT(ISERROR(SEARCH("Playing",D1)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="14" priority="48" operator="beginsWith" text="Played">
+      <formula>LEFT(D1,LEN("Played"))="Played"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="49" operator="containsText" text="Ignore">
+      <formula>NOT(ISERROR(SEARCH("Ignore",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="50" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="51" operator="containsText" text="Quit">
+      <formula>NOT(ISERROR(SEARCH("Quit",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -896,99 +925,74 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="8.85546875" customWidth="1" style="3" min="1" max="1"/>
-    <col width="54.28515625" customWidth="1" style="4" min="2" max="2"/>
-    <col width="9.28515625" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
-    <col width="9.140625" customWidth="1" style="2" min="4" max="16384"/>
+    <col min="1" max="1" width="8.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="72" customFormat="1" customHeight="1" s="1" thickBot="1">
-      <c r="A1" s="7" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="6" t="inlineStr">
-        <is>
-          <t>Birth Month</t>
-        </is>
-      </c>
-      <c r="C1" s="9" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="10" t="inlineStr">
-        <is>
-          <t>Michael</t>
-        </is>
-      </c>
-      <c r="B2" s="11" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-      <c r="C2" s="8" t="n">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="8">
         <v>31</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="10" t="inlineStr">
-        <is>
-          <t>Brian</t>
-        </is>
-      </c>
-      <c r="B3" s="11" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-      <c r="C3" s="8" t="n">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="8">
         <v>33</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="10" t="inlineStr">
-        <is>
-          <t>Allison</t>
-        </is>
-      </c>
-      <c r="B4" s="11" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-      <c r="C4" s="8" t="n">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="8">
         <v>34</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="10" t="inlineStr">
-        <is>
-          <t>Rob</t>
-        </is>
-      </c>
-      <c r="B5" s="11" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-      <c r="C5" s="8" t="n">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="8">
         <v>36</v>
       </c>
     </row>
@@ -1006,40 +1010,96 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="10">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"Endless"</formula>
     </cfRule>
-    <cfRule type="containsText" priority="2" operator="containsText" dxfId="9" text="Removed">
+    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="Removed">
       <formula>NOT(ISERROR(SEARCH("Removed",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="3" operator="containsText" dxfId="8" text="Software">
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Software">
       <formula>NOT(ISERROR(SEARCH("Software",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="4" operator="containsText" dxfId="7" text="Demo">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="Demo">
       <formula>NOT(ISERROR(SEARCH("Demo",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="5" operator="containsText" dxfId="6" text="Waiting">
+    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="Waiting">
       <formula>NOT(ISERROR(SEARCH("Waiting",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="6" operator="containsText" dxfId="5" text="Unplayed">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Unplayed">
       <formula>NOT(ISERROR(SEARCH("Unplayed",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="7" operator="containsText" dxfId="3" text="Playing">
+    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="Playing">
       <formula>NOT(ISERROR(SEARCH("Playing",C1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" priority="8" operator="beginsWith" dxfId="3" text="Played">
+    <cfRule type="beginsWith" dxfId="3" priority="8" operator="beginsWith" text="Played">
       <formula>LEFT(C1,LEN("Played"))="Played"</formula>
     </cfRule>
-    <cfRule type="containsText" priority="9" operator="containsText" dxfId="2" text="Ignore">
+    <cfRule type="containsText" dxfId="2" priority="9" operator="containsText" text="Ignore">
       <formula>NOT(ISERROR(SEARCH("Ignore",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="10" operator="containsText" dxfId="1" text="Finished">
+    <cfRule type="containsText" dxfId="1" priority="10" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="11" operator="containsText" dxfId="0" text="Quit">
+    <cfRule type="containsText" dxfId="0" priority="11" operator="containsText" text="Quit">
       <formula>NOT(ISERROR(SEARCH("Quit",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="12" t="str">
+        <f>HYPERLINK("https://www.Stark.com/","Website")</f>
+        <v>Website</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:A2">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="10"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
 </file>
</xml_diff>